<commit_message>
export eduprog to excel rework
</commit_message>
<xml_diff>
--- a/CompetenciesMatrix.xlsx
+++ b/CompetenciesMatrix.xlsx
@@ -4,48 +4,61 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="true" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Перелік компонент" sheetId="1" r:id="rId1"/>
+    <sheet name="Матриця компетентностей" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>Код н/д</t>
+  </si>
+  <si>
+    <t>Компоненти освітньої програми (навчальні дисципліни, курсові проекти (роботи), практики, кваліфікаційна робота)</t>
+  </si>
+  <si>
+    <t>Кількість кредитів</t>
+  </si>
+  <si>
+    <t>Форма підсумкового контролю</t>
+  </si>
+  <si>
+    <t>Обов'язкові компоненти ОП</t>
+  </si>
+  <si>
+    <t>ОК 1.</t>
+  </si>
+  <si>
+    <t>fавіаdaвіаfsaf</t>
+  </si>
+  <si>
+    <t>залік</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Загальний обсяг обов'язкових компонент: </t>
+  </si>
+  <si>
+    <t>10 кредитів</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Загальний обсяг вибіркових компонент: </t>
+  </si>
+  <si>
+    <t>0 кредитів</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ЗАГАЛЬНИЙ ОБСЯГ ОСВІТНЬОЇ ПРОГРАМИ: </t>
+  </si>
   <si>
     <t>ОК 1</t>
   </si>
   <si>
-    <t>ОК 2</t>
-  </si>
-  <si>
-    <t>ОК 3</t>
-  </si>
-  <si>
-    <t>ОК 4</t>
-  </si>
-  <si>
-    <t>ОК 5</t>
-  </si>
-  <si>
-    <t>ОК 6</t>
-  </si>
-  <si>
-    <t>ОК 7</t>
-  </si>
-  <si>
-    <t>ОК 8</t>
-  </si>
-  <si>
-    <t>ОК 9</t>
-  </si>
-  <si>
-    <t>ОК 10</t>
-  </si>
-  <si>
     <t>ЗК 1</t>
   </si>
   <si>
@@ -53,44 +66,23 @@
   </si>
   <si>
     <t>ЗК 3</t>
-  </si>
-  <si>
-    <t>ЗК 4</t>
-  </si>
-  <si>
-    <t>ЗК 5</t>
-  </si>
-  <si>
-    <t>ЗК 6</t>
-  </si>
-  <si>
-    <t>ЗК 7</t>
-  </si>
-  <si>
-    <t>ЗК 8</t>
-  </si>
-  <si>
-    <t>ЗК 9</t>
-  </si>
-  <si>
-    <t>ЗК 10</t>
-  </si>
-  <si>
-    <t>ЗК 11</t>
-  </si>
-  <si>
-    <t>·</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color/>
+      <name val="Times New Roman"/>
       <family val="2"/>
     </font>
     <font>
@@ -143,15 +135,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" textRotation="90" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -423,221 +424,141 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" max="11" min="2" width="3"/>
+    <col customWidth="true" max="1" min="1" width="10"/>
+    <col customWidth="true" max="2" min="2" width="50"/>
+    <col customWidth="true" max="3" min="3" width="15"/>
+    <col customWidth="true" max="4" min="4" width="20"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+  </mergeCells>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="true" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col customWidth="true" max="2" min="2" width="3"/>
   </cols>
   <sheetData>
     <row r="1" ht="40" customHeight="true">
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
+      <c r="B1" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="true">
       <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="B2" s="6"/>
     </row>
     <row r="3" ht="15" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="B3" s="6"/>
     </row>
     <row r="4" ht="15" customHeight="true">
       <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" ht="15" customHeight="true">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" ht="15" customHeight="true">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" ht="15" customHeight="true">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" ht="15" customHeight="true">
-      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" ht="15" customHeight="true">
-      <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" ht="15" customHeight="true">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" ht="15" customHeight="true">
-      <c r="A11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" ht="15" customHeight="true">
-      <c r="A12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="B4" s="6"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>